<commit_message>
Fixed typo in Fig. 10
</commit_message>
<xml_diff>
--- a/paper/pldi23/img/data.xlsx
+++ b/paper/pldi23/img/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/naldo/project/internal-esmeta/babel-study/paper/pldi23/img/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CA55483-E05A-2141-8D59-BF11A851210C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E247FB4-92C7-2148-BC49-6B307330B263}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" activeTab="1" xr2:uid="{45A293A3-4F51-A547-B5E2-28579CD7826C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" activeTab="2" xr2:uid="{45A293A3-4F51-A547-B5E2-28579CD7826C}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -5898,7 +5898,7 @@
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
                   </a:rPr>
-                  <a:t> 1-FCPS-TP</a:t>
+                  <a:t> 1-FCPS-TR</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-US" sz="1800">
                   <a:solidFill>
@@ -6952,7 +6952,7 @@
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
                   </a:rPr>
-                  <a:t> 2-FS-TP</a:t>
+                  <a:t> 2-FS-TR</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-US" sz="1800">
                   <a:solidFill>
@@ -8006,7 +8006,7 @@
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
                   </a:rPr>
-                  <a:t> 2-FCPS-TP</a:t>
+                  <a:t> 2-FCPS-TR</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-US" sz="1800">
                   <a:solidFill>
@@ -9060,7 +9060,7 @@
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
                   </a:rPr>
-                  <a:t> 1-FS-TP</a:t>
+                  <a:t> 1-FS-TR</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-US" sz="1800">
                   <a:solidFill>
@@ -10114,7 +10114,7 @@
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
                   </a:rPr>
-                  <a:t> 0-FS-TP</a:t>
+                  <a:t> 0-FS-TR</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-US" sz="1800">
                   <a:solidFill>
@@ -24919,8 +24919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A482B568-3A2B-BA4B-AD64-D5FFA86816B5}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="158" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView zoomScale="158" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -24935,8 +24935,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B79D6C58-FFF6-5E4B-A1D1-27DBF53CA5CB}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScale="135" zoomScaleNormal="138" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" zoomScale="135" zoomScaleNormal="138" workbookViewId="0">
+      <selection activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>